<commit_message>
fixed units issued of gauss and Si
</commit_message>
<xml_diff>
--- a/magnetic_mapping.xlsx
+++ b/magnetic_mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="0" windowWidth="25040" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="500" yWindow="0" windowWidth="25040" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -442,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O199"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="C106" workbookViewId="0">
+      <selection activeCell="I72" sqref="I72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2839,7 +2839,7 @@
         <v>0.26200000000000001</v>
       </c>
       <c r="I68">
-        <v>334</v>
+        <v>0.33400000000000002</v>
       </c>
       <c r="J68">
         <v>0.44900000000000001</v>
@@ -5225,7 +5225,7 @@
         <v>7.25</v>
       </c>
       <c r="C128">
-        <v>3.6</v>
+        <v>0.36</v>
       </c>
       <c r="D128">
         <v>0.38</v>
@@ -5273,7 +5273,7 @@
         <v>8.25</v>
       </c>
       <c r="C129">
-        <v>3.2949999999999999</v>
+        <v>0.32950000000000002</v>
       </c>
       <c r="D129">
         <v>0.36599999999999999</v>

</xml_diff>

<commit_message>
check to see if electron is caught in loop
</commit_message>
<xml_diff>
--- a/magnetic_mapping.xlsx
+++ b/magnetic_mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="0" windowWidth="25040" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="1880" yWindow="2820" windowWidth="28140" windowHeight="17700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -442,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C106" workbookViewId="0">
-      <selection activeCell="I72" sqref="I72"/>
+    <sheetView tabSelected="1" topLeftCell="C115" workbookViewId="0">
+      <selection activeCell="N74" sqref="N74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -675,7 +675,7 @@
         <v>0.58499999999999996</v>
       </c>
       <c r="N8">
-        <v>610</v>
+        <v>0.61</v>
       </c>
       <c r="O8">
         <v>0.496</v>
@@ -723,7 +723,7 @@
         <v>0.71899999999999997</v>
       </c>
       <c r="N9">
-        <v>741</v>
+        <v>0.74099999999999999</v>
       </c>
       <c r="O9">
         <v>0.59199999999999997</v>
@@ -3136,7 +3136,7 @@
         <v>0.68700000000000006</v>
       </c>
       <c r="L74">
-        <v>719</v>
+        <v>0.71899999999999997</v>
       </c>
       <c r="M74">
         <v>0.68200000000000005</v>
@@ -4563,7 +4563,7 @@
         <v>0.27800000000000002</v>
       </c>
       <c r="L109">
-        <v>290</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="M109">
         <v>0.27600000000000002</v>
@@ -5396,7 +5396,7 @@
         <v>0.68300000000000005</v>
       </c>
       <c r="L131">
-        <v>768</v>
+        <v>0.76800000000000002</v>
       </c>
       <c r="M131">
         <v>0.76800000000000002</v>

</xml_diff>